<commit_message>
Error correction in function transposer (RowFilter not run)
</commit_message>
<xml_diff>
--- a/inst/extdata/ERD_UG_Example_1_v10.xlsx
+++ b/inst/extdata/ERD_UG_Example_1_v10.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="87">
   <si>
     <t xml:space="preserve">TableName </t>
   </si>
@@ -320,34 +320,25 @@
     <t xml:space="preserve">DataType</t>
   </si>
   <si>
-    <t xml:space="preserve">dateEstimationType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dateMissingType </t>
-  </si>
-  <si>
     <t xml:space="preserve">INDIV_INDIV</t>
   </si>
   <si>
+    <t xml:space="preserve">"Husband"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Wife"</t>
+  </si>
+  <si>
     <t xml:space="preserve">dadid</t>
   </si>
   <si>
+    <t xml:space="preserve">"Father"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Child"</t>
+  </si>
+  <si>
     <t xml:space="preserve">momid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Husband"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Wife"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Father"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Time_Invariant"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Child"</t>
   </si>
   <si>
     <t xml:space="preserve">"Mother"</t>
@@ -381,7 +372,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -435,6 +426,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -533,7 +530,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -571,31 +568,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -680,7 +677,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1612,7 +1609,7 @@
   <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1669,88 +1666,94 @@
         <v>71</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
     </row>
-    <row r="2" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="9"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="7"/>
+      <c r="L2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="9"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="7"/>
+      <c r="L3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -1760,33 +1763,35 @@
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="9"/>
+      <c r="E4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="13"/>
       <c r="J4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="9"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="13"/>
       <c r="M4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N4" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
@@ -1796,33 +1801,35 @@
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="9"/>
+      <c r="E5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="9"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N5" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
@@ -1832,325 +1839,355 @@
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="9"/>
+      <c r="E6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="13"/>
       <c r="J6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="9"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="13"/>
       <c r="M6" s="1" t="s">
-        <v>80</v>
+        <v>27</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="9"/>
+      <c r="D7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="9"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="E8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="12"/>
+      <c r="L8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="A9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="E9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="12"/>
+      <c r="L9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="E10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="12"/>
+      <c r="L10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="D11" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="1" t="s">
-        <v>80</v>
+        <v>27</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="12"/>
+      <c r="L12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K13" s="13" t="s">
+      <c r="D14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="12"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="12" t="s">
+      <c r="L14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="12"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="12"/>
+      <c r="L15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="N15" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Minor corrections in variable names
</commit_message>
<xml_diff>
--- a/inst/extdata/ERD_UG_Example_1_v10.xlsx
+++ b/inst/extdata/ERD_UG_Example_1_v10.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="84">
   <si>
     <t xml:space="preserve">TableName </t>
   </si>
@@ -308,15 +308,6 @@
     <t xml:space="preserve">ToEntityID</t>
   </si>
   <si>
-    <t xml:space="preserve">VariableName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expression</t>
-  </si>
-  <si>
     <t xml:space="preserve">DataType</t>
   </si>
   <si>
@@ -372,7 +363,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -426,12 +417,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -530,7 +515,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -576,24 +561,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1606,591 +1591,537 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S1048576"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="13" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="J1" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="1" t="s">
+      <c r="F2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="J2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="1" t="s">
+      <c r="F3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="J3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="F4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="1" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="F5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="1" t="s">
+      <c r="J5" s="14"/>
+      <c r="K5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="F6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="1" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="E7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="1" t="s">
+      <c r="J7" s="14"/>
+      <c r="K7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="1" t="s">
+      <c r="F8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="I8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="J8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="1" t="s">
+      <c r="F9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="J9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="1" t="s">
+      <c r="F10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="J10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>81</v>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="I11" s="8"/>
-      <c r="J11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="1" t="s">
+      <c r="J11" s="8"/>
+      <c r="K11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="I12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="8"/>
-      <c r="N12" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="J12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" s="14" t="s">
+      <c r="H13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="8"/>
-      <c r="N13" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="J13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K14" s="14" t="s">
+      <c r="H14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="J14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="I15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="J15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="8"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>